<commit_message>
minor improvements to HeapTest and charts
</commit_message>
<xml_diff>
--- a/aisd_lab_1_sorting/graphs.xlsx
+++ b/aisd_lab_1_sorting/graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\materialy\III-sem\astruk\laby\lab01\astrukNauka\2021Z_AISD_lab_git_gr6\aisd_lab_1_sorting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52C58C19-1816-48A9-A209-D7DB47610F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B189470-1559-4A94-A645-B8D675E7C69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C8219043-E25A-4908-A49C-CDC7DDFE3361}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8DC825C1-F792-4EE7-8F91-A7F1126B16D3}"/>
   </bookViews>
   <sheets>
     <sheet name="combined" sheetId="1" r:id="rId1"/>
@@ -3574,7 +3574,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5258-49F8-AEAC-62C562F22B2B}"/>
+              <c16:uniqueId val="{00000000-CE26-4D53-953B-A53AC9C8EBB7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4310,7 +4310,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4444-4C77-8B4F-71466BB63392}"/>
+              <c16:uniqueId val="{00000000-55AA-4C53-991D-BC1A9BD7D2D6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5048,7 +5048,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D182-441C-908D-C9FE4BA16A34}"/>
+              <c16:uniqueId val="{00000000-8DD8-4597-9958-245B52089AF7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5481,7 +5481,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D182-441C-908D-C9FE4BA16A34}"/>
+              <c16:uniqueId val="{00000001-8DD8-4597-9958-245B52089AF7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5914,7 +5914,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D182-441C-908D-C9FE4BA16A34}"/>
+              <c16:uniqueId val="{00000002-8DD8-4597-9958-245B52089AF7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6680,7 +6680,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-54C1-46F9-9230-4E648D421427}"/>
+              <c16:uniqueId val="{00000000-34B8-4BF9-A474-3A119BEADA97}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7113,7 +7113,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-54C1-46F9-9230-4E648D421427}"/>
+              <c16:uniqueId val="{00000001-34B8-4BF9-A474-3A119BEADA97}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7546,7 +7546,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-54C1-46F9-9230-4E648D421427}"/>
+              <c16:uniqueId val="{00000002-34B8-4BF9-A474-3A119BEADA97}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7979,7 +7979,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-54C1-46F9-9230-4E648D421427}"/>
+              <c16:uniqueId val="{00000003-34B8-4BF9-A474-3A119BEADA97}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8742,7 +8742,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1C39-484F-A41E-A11EAD1133C2}"/>
+              <c16:uniqueId val="{00000000-16C9-4652-955B-60DDF55D42F3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8761,6 +8761,7 @@
         <c:axId val="148420512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="50000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -9479,7 +9480,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D785-4740-AE2B-4D2B0EE65DC3}"/>
+              <c16:uniqueId val="{00000000-57A2-4BC4-8020-D2A5E5D728C4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9912,7 +9913,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D785-4740-AE2B-4D2B0EE65DC3}"/>
+              <c16:uniqueId val="{00000001-57A2-4BC4-8020-D2A5E5D728C4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10345,7 +10346,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D785-4740-AE2B-4D2B0EE65DC3}"/>
+              <c16:uniqueId val="{00000002-57A2-4BC4-8020-D2A5E5D728C4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10778,7 +10779,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D785-4740-AE2B-4D2B0EE65DC3}"/>
+              <c16:uniqueId val="{00000003-57A2-4BC4-8020-D2A5E5D728C4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -11541,7 +11542,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DC0D-434C-9EF7-8A0FB3035C17}"/>
+              <c16:uniqueId val="{00000000-19D0-4B53-A61B-E88331786DB1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12277,7 +12278,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A8AD-4664-A67C-17A7FF1066D1}"/>
+              <c16:uniqueId val="{00000000-C8D7-46D7-96B7-68936432C202}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13012,7 +13013,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6A62-455B-91EA-33ED131A121A}"/>
+              <c16:uniqueId val="{00000000-24A1-4495-B93C-661B3E03D183}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13140,6 +13141,7 @@
         <c:axId val="167838544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="500000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -13747,7 +13749,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D9EE-4ECF-BBAA-688B3AE7D343}"/>
+              <c16:uniqueId val="{00000000-67C6-434C-8B96-EF819109157A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -14483,7 +14485,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A428-4A55-A310-1BCEE02CE8E8}"/>
+              <c16:uniqueId val="{00000000-B2BF-4710-9637-538C40F34B0B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -17918,7 +17920,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9828-430C-AF3E-2CA7E3B75345}"/>
+              <c16:uniqueId val="{00000000-1247-4D05-AF93-1806476D7CEB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -18653,7 +18655,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A32F-49EF-9E31-B2939D1A3DAE}"/>
+              <c16:uniqueId val="{00000000-8859-4491-93B6-F78CEBB9D086}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -19389,7 +19391,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2FB2-49B7-A909-9AE35E28B94A}"/>
+              <c16:uniqueId val="{00000000-4560-4B90-A4F3-3D7D635214DD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -27482,7 +27484,7 @@
         <xdr:cNvPr id="2" name="Wykres 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{422961F0-470B-468F-8111-BD0FAAA068F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A98EF1FB-38FB-4EED-9147-CB91B5C9E6F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27520,7 +27522,7 @@
         <xdr:cNvPr id="3" name="Wykres 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C1DA27D-C0BB-448C-9401-E6D651F477E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7433A7F-715E-4394-A765-EE98987C5478}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27558,7 +27560,7 @@
         <xdr:cNvPr id="4" name="Wykres 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DA3BF22-D30E-4BD4-AD37-267D4F77909C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54DCBD8E-F10A-4E31-B3EF-EF9E1154EF3D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27596,7 +27598,7 @@
         <xdr:cNvPr id="5" name="Wykres 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{945B17C4-773C-448C-BDD7-4E22CAD16C52}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35E276F5-5229-4D40-833D-5B80AB37E714}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27634,7 +27636,7 @@
         <xdr:cNvPr id="6" name="Wykres 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{253C7C5E-26B3-4EA9-B570-43285194407A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0953F7A2-1ECA-41FB-8B70-E1A0ED1845D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27672,7 +27674,7 @@
         <xdr:cNvPr id="7" name="Wykres 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BE66556-9139-4B0A-B21F-87757ED38ABE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B602A4FC-4243-42BE-990E-0E479D2ADD3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27710,7 +27712,7 @@
         <xdr:cNvPr id="8" name="Wykres 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C13A771-3A0C-4E7B-BF98-FA0468C856D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26268278-092B-4B2A-B74D-4E1BDA24E7B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27748,7 +27750,7 @@
         <xdr:cNvPr id="9" name="Wykres 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B7A3CFF-0EC4-40F0-8FAE-6D8D6F0ED397}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01E12310-026F-4BFF-9B8E-3685EE0C951B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27786,7 +27788,7 @@
         <xdr:cNvPr id="10" name="Wykres 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{868A7092-17A1-4866-A7BA-755C1FB470ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB3819BC-8691-4B41-B47F-DE40CEB38D2F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27824,7 +27826,7 @@
         <xdr:cNvPr id="11" name="Wykres 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0768C441-410B-418D-BED1-DC85C251EAD8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A40719F6-9E79-4D4D-BDFA-8DCE446F2659}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27862,7 +27864,7 @@
         <xdr:cNvPr id="12" name="Wykres 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADD67FF4-F2EE-4BD5-A71E-F5AD94853258}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A4EFA71-A95F-40B3-B6F1-05E48941119B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27900,7 +27902,7 @@
         <xdr:cNvPr id="13" name="Wykres 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B02E0B3-C385-4A32-B29F-8C365A22244B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D69601C4-45E3-4EA9-85AE-363C62185CEB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27938,7 +27940,7 @@
         <xdr:cNvPr id="14" name="Wykres 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE894AE0-0BD6-4B36-AA8E-CCA46064A3DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7917D628-28FC-43A0-92C1-A6DF05D3BBA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27976,7 +27978,7 @@
         <xdr:cNvPr id="15" name="Wykres 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC612AC0-B250-4C85-804E-8DCD5B36BE84}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BBC587D-651E-41DB-B4B7-ECDDC86DB05D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28011,6 +28013,7 @@
       <sheetName val="worstCaseCombined"/>
       <sheetName val="randomCombined"/>
       <sheetName val="combined"/>
+      <sheetName val="test"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -43818,6 +43821,7 @@
         </row>
       </sheetData>
       <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -44119,11 +44123,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344D90F0-DA61-4E9D-AF19-095AFB2EB94A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD090B03-968F-4D54-A3DC-9B1BEF3E5576}">
   <dimension ref="A1:AQ57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG27" sqref="AG27"/>
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
heap is now type of HeapInterface
</commit_message>
<xml_diff>
--- a/aisd_lab_1_sorting/graphs.xlsx
+++ b/aisd_lab_1_sorting/graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\materialy\III-sem\astruk\laby\lab01\astrukNauka\2021Z_AISD_lab_git_gr6\aisd_lab_1_sorting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A86C3350-6873-4825-BD7D-BCC1765C9CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9AF81D7-C215-439E-ADB0-CDA3E94BC99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2190B6FD-219E-4B80-9320-BD83C794FE87}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{748AB17B-DCEC-430B-9FB9-8D0E39E7B054}"/>
   </bookViews>
   <sheets>
     <sheet name="combined" sheetId="1" r:id="rId1"/>
@@ -3588,7 +3588,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5BA5-4871-BB5C-16BD425BF7A7}"/>
+              <c16:uniqueId val="{00000000-BDB7-4819-BC13-37093DE11EAA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3751,9 +3751,22 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:rPr lang="pl-PL" b="0"/>
+                  <a:t>Czas [</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" b="0"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4327,7 +4340,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AB87-4F80-9DF9-9A1A6FC6A448}"/>
+              <c16:uniqueId val="{00000000-AC67-485D-8E07-FF402C2401E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4760,7 +4773,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AB87-4F80-9DF9-9A1A6FC6A448}"/>
+              <c16:uniqueId val="{00000001-AC67-485D-8E07-FF402C2401E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5193,7 +5206,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-AB87-4F80-9DF9-9A1A6FC6A448}"/>
+              <c16:uniqueId val="{00000002-AC67-485D-8E07-FF402C2401E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5626,7 +5639,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-AB87-4F80-9DF9-9A1A6FC6A448}"/>
+              <c16:uniqueId val="{00000003-AC67-485D-8E07-FF402C2401E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5789,7 +5802,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6389,7 +6410,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6037-4B7C-A578-9005E0094E1A}"/>
+              <c16:uniqueId val="{00000000-DE60-4387-A5FE-2BD593494CCE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6552,7 +6573,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -7127,7 +7156,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0185-4350-87A6-0721E49549F9}"/>
+              <c16:uniqueId val="{00000000-4538-4D3F-BD21-BD74ED47A0A1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7560,7 +7589,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0185-4350-87A6-0721E49549F9}"/>
+              <c16:uniqueId val="{00000001-4538-4D3F-BD21-BD74ED47A0A1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7993,7 +8022,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0185-4350-87A6-0721E49549F9}"/>
+              <c16:uniqueId val="{00000002-4538-4D3F-BD21-BD74ED47A0A1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8426,7 +8455,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-0185-4350-87A6-0721E49549F9}"/>
+              <c16:uniqueId val="{00000003-4538-4D3F-BD21-BD74ED47A0A1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8589,7 +8618,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -11889,7 +11926,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7AA4-4D15-9146-1DA48386AEBF}"/>
+              <c16:uniqueId val="{00000000-E661-4572-9FF2-289D1F77D240}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12052,7 +12089,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -12624,7 +12669,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-34E6-4964-A477-F098DD5DC850}"/>
+              <c16:uniqueId val="{00000000-8281-409D-A794-26F1168A9454}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12787,7 +12832,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -13362,7 +13415,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4E84-452F-B9E1-C2B015097437}"/>
+              <c16:uniqueId val="{00000000-8120-41E0-95D4-FCEE0F4D4E0E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13795,7 +13848,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4E84-452F-B9E1-C2B015097437}"/>
+              <c16:uniqueId val="{00000001-8120-41E0-95D4-FCEE0F4D4E0E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -14228,7 +14281,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4E84-452F-B9E1-C2B015097437}"/>
+              <c16:uniqueId val="{00000002-8120-41E0-95D4-FCEE0F4D4E0E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -14661,7 +14714,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-4E84-452F-B9E1-C2B015097437}"/>
+              <c16:uniqueId val="{00000003-8120-41E0-95D4-FCEE0F4D4E0E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -14824,7 +14877,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -15424,7 +15485,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-85F0-460B-B860-DA7DFD01701A}"/>
+              <c16:uniqueId val="{00000000-8E0F-4DF9-8CBE-E0C5B423F43A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15588,7 +15649,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -16160,7 +16229,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3410-4F81-9B1A-DD56A5652A6E}"/>
+              <c16:uniqueId val="{00000000-E034-4DD8-A227-E2874632916D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -16324,7 +16393,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -16896,7 +16973,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-74AB-4F56-8B79-9D15DFAE0972}"/>
+              <c16:uniqueId val="{00000000-DE84-4214-BC8D-CB039219B8A5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -17060,7 +17137,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -17632,7 +17717,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D1EF-4E85-9C72-2860666C9C2E}"/>
+              <c16:uniqueId val="{00000000-333D-4B32-B244-590A06D8CCFE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -17796,7 +17881,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -21068,7 +21161,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AF18-4BDA-A6D0-6516164B33D8}"/>
+              <c16:uniqueId val="{00000000-B114-4E3B-ACF9-9D94F32C6552}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -21231,7 +21324,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -21803,7 +21904,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-877B-48EE-B98A-C91CA786BAB8}"/>
+              <c16:uniqueId val="{00000000-7B73-4BE1-ADCE-E12D039CCE4F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -21967,7 +22068,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -22539,7 +22648,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2DD8-40F6-ABF3-D168C8182785}"/>
+              <c16:uniqueId val="{00000000-C9BC-4935-8523-A01F14880414}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -22702,7 +22811,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -23274,7 +23391,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4F91-4FA8-B4F5-F9146F8EC391}"/>
+              <c16:uniqueId val="{00000000-3C8F-434A-81A0-4564C92CB141}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -23437,7 +23554,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Mikrosekundy</a:t>
+                  <a:t>Czas [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -31923,7 +32048,7 @@
         <xdr:cNvPr id="2" name="Wykres 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C6E2F7-78D4-420D-9E4E-0EFB2C6EAD0E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31A2B5E5-9EE8-4073-80DA-BB10098096BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31961,7 +32086,7 @@
         <xdr:cNvPr id="3" name="Wykres 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F60301E-EA32-47B9-BB8C-45D7340DE1AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C19E5F0D-3E29-46B2-BA3B-4E0D75BC13D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31999,7 +32124,7 @@
         <xdr:cNvPr id="4" name="Wykres 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC5B725C-8181-407B-A8EA-A6F12E107BC0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0708FEB-2D5B-486A-A7AF-93709358A890}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32037,7 +32162,7 @@
         <xdr:cNvPr id="5" name="Wykres 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87BB1B51-694F-4E83-A79A-931985220489}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{253EB036-3FEA-4B96-B698-98CD8DA55785}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32075,7 +32200,7 @@
         <xdr:cNvPr id="6" name="Wykres 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A30CDAEB-637F-4186-86B5-130E9CD94D76}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46378AF8-FCB5-48BA-80F1-56DBE616FCC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32113,7 +32238,7 @@
         <xdr:cNvPr id="7" name="Wykres 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A3BF047-ABED-4E63-894B-088DCE783232}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D4FC92B-CB27-46C0-8D49-EBC12E2FEB3F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32151,7 +32276,7 @@
         <xdr:cNvPr id="8" name="Wykres 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4CB702A-8DDA-44F6-B943-82478244A68C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3072AB20-0323-4787-A8DC-95C7B0A8B3D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32189,7 +32314,7 @@
         <xdr:cNvPr id="9" name="Wykres 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9803A213-860E-420D-9438-447C5A335309}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFE88DF1-D6C3-4CFA-AC35-0D509BCB3719}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32227,7 +32352,7 @@
         <xdr:cNvPr id="10" name="Wykres 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CA1B3F5-95D5-4BAE-864F-9E5A53B0AB86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BBD3CB-A6C3-404D-9E5B-B4D453DD84B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32265,7 +32390,7 @@
         <xdr:cNvPr id="11" name="Wykres 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDBD8D05-0503-42A7-AAB6-D878FDDC9C0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B2EC198-6C80-49AC-A313-EC1A8D593394}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32303,7 +32428,7 @@
         <xdr:cNvPr id="12" name="Wykres 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F145CF2F-5411-4400-BDD7-49CEFA6C3C07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1872C36B-8720-406F-B443-134B3B5F4FEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32341,7 +32466,7 @@
         <xdr:cNvPr id="13" name="Wykres 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC9D2180-D90D-4CC3-B219-66687300882C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9E20EEB-5C5C-4B52-8FB8-E6BD2C6D577F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32379,7 +32504,7 @@
         <xdr:cNvPr id="14" name="Wykres 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4CFE8C6-B13A-40BD-85E5-4EB5B9DACD52}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95879415-5031-4FFF-8EF3-429057B383D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32417,7 +32542,7 @@
         <xdr:cNvPr id="15" name="Wykres 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9314DC5-268C-416A-9DA8-A27FFF1F0ED6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13F56FE3-773F-4954-B430-50300706E209}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32455,7 +32580,7 @@
         <xdr:cNvPr id="16" name="Wykres 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E437AC3F-16A9-4ED6-988B-D49CAAAB1674}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00D55F19-9B90-4F70-B37E-78B5C097314A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -52980,11 +53105,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9301C265-1BE1-4079-BA32-FABED303B35A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184B5735-7F4A-4259-9088-C2EE0EA69FC2}">
   <dimension ref="A1:AQ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AS10" sqref="AS10"/>
+    <sheetView tabSelected="1" topLeftCell="X25" workbookViewId="0">
+      <selection activeCell="AR43" sqref="AR43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>